<commit_message>
Updated Locator to play with climber
</commit_message>
<xml_diff>
--- a/IO Assignment.xlsx
+++ b/IO Assignment.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="17040" windowHeight="9210"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
   <si>
     <t>PWM Outputs</t>
   </si>
@@ -199,13 +199,25 @@
   </si>
   <si>
     <t>Bobcat 2013 IO Assignments</t>
+  </si>
+  <si>
+    <t>Upper Limit Switch</t>
+  </si>
+  <si>
+    <t>Lower Limit Switch</t>
+  </si>
+  <si>
+    <t>Shooter Encoder A</t>
+  </si>
+  <si>
+    <t>Shooter Encoder B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,7 +264,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -449,11 +461,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -528,12 +551,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -612,6 +641,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -646,6 +676,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -821,17 +852,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.25" customWidth="1"/>
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
@@ -846,7 +877,7 @@
     <col min="14" max="14" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="23.25">
+    <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="29" t="s">
         <v>59</v>
       </c>
@@ -865,7 +896,7 @@
       <c r="N1" s="30"/>
       <c r="O1" s="30"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -882,7 +913,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="15" thickBot="1">
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -899,7 +930,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" ht="15">
+    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>0</v>
       </c>
@@ -926,7 +957,7 @@
       <c r="N4" s="28"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -959,7 +990,7 @@
       <c r="N5" s="5"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -996,7 +1027,7 @@
       </c>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>3</v>
       </c>
@@ -1027,7 +1058,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>4</v>
       </c>
@@ -1058,7 +1089,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>5</v>
       </c>
@@ -1091,7 +1122,7 @@
       </c>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:15" ht="15" thickBot="1">
+    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>6</v>
       </c>
@@ -1120,7 +1151,7 @@
       <c r="N10" s="7"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>7</v>
       </c>
@@ -1145,7 +1176,7 @@
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="12" spans="1:15" ht="15.75" thickBot="1">
+    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>8</v>
       </c>
@@ -1170,7 +1201,7 @@
       <c r="N12" s="10"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>9</v>
       </c>
@@ -1189,7 +1220,7 @@
       <c r="N13" s="9"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="1:15" ht="15" thickBot="1">
+    <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>10</v>
       </c>
@@ -1208,7 +1239,7 @@
       <c r="N14" s="9"/>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="1:15" ht="15" thickBot="1">
+    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1225,7 +1256,7 @@
       <c r="N15" s="9"/>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="1:15" ht="15">
+    <row r="16" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>1</v>
       </c>
@@ -1250,7 +1281,7 @@
       <c r="N16" s="9"/>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>1</v>
       </c>
@@ -1281,7 +1312,7 @@
       <c r="N17" s="9"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>2</v>
       </c>
@@ -1308,7 +1339,7 @@
       <c r="N18" s="9"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>3</v>
       </c>
@@ -1335,7 +1366,7 @@
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" spans="1:15" ht="15">
+    <row r="20" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>4</v>
       </c>
@@ -1362,7 +1393,7 @@
       <c r="N20" s="10"/>
       <c r="O20" s="2"/>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>5</v>
       </c>
@@ -1387,11 +1418,13 @@
       <c r="N21" s="9"/>
       <c r="O21" s="2"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>6</v>
       </c>
-      <c r="B22" s="5"/>
+      <c r="B22" s="32" t="s">
+        <v>62</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="4">
         <v>6</v>
@@ -1410,11 +1443,13 @@
       <c r="N22" s="9"/>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>7</v>
       </c>
-      <c r="B23" s="5"/>
+      <c r="B23" s="32" t="s">
+        <v>63</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="4">
         <v>7</v>
@@ -1433,11 +1468,13 @@
       <c r="N23" s="9"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" spans="1:15" ht="15" thickBot="1">
+    <row r="24" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>8</v>
       </c>
-      <c r="B24" s="5"/>
+      <c r="B24" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="6">
         <v>8</v>
@@ -1456,11 +1493,13 @@
       <c r="N24" s="9"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>9</v>
       </c>
-      <c r="B25" s="5"/>
+      <c r="B25" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1477,7 +1516,7 @@
       <c r="N25" s="9"/>
       <c r="O25" s="2"/>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>10</v>
       </c>
@@ -1498,7 +1537,7 @@
       <c r="N26" s="9"/>
       <c r="O26" s="2"/>
     </row>
-    <row r="27" spans="1:15" ht="15" thickBot="1">
+    <row r="27" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>11</v>
       </c>
@@ -1519,7 +1558,7 @@
       <c r="N27" s="9"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="1:15" ht="15">
+    <row r="28" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>12</v>
       </c>
@@ -1542,7 +1581,7 @@
       <c r="N28" s="9"/>
       <c r="O28" s="2"/>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>13</v>
       </c>
@@ -1567,7 +1606,7 @@
       <c r="N29" s="9"/>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" spans="1:15" ht="15" thickBot="1">
+    <row r="30" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>14</v>
       </c>
@@ -1590,7 +1629,7 @@
       <c r="N30" s="9"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" spans="1:15" ht="15" thickBot="1">
+    <row r="31" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1611,7 +1650,7 @@
       <c r="N31" s="9"/>
       <c r="O31" s="2"/>
     </row>
-    <row r="32" spans="1:15" ht="15.75" thickBot="1">
+    <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="25" t="s">
         <v>25</v>
       </c>
@@ -1634,7 +1673,7 @@
       <c r="N32" s="9"/>
       <c r="O32" s="2"/>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>1</v>
       </c>
@@ -1657,7 +1696,7 @@
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
     </row>
-    <row r="34" spans="1:15" ht="15" thickBot="1">
+    <row r="34" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>2</v>
       </c>
@@ -1678,7 +1717,7 @@
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>3</v>
       </c>
@@ -1697,7 +1736,7 @@
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>4</v>
       </c>
@@ -1716,7 +1755,7 @@
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
     </row>
-    <row r="37" spans="1:15" ht="15" thickBot="1">
+    <row r="37" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>5</v>
       </c>
@@ -1735,7 +1774,7 @@
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1752,7 +1791,7 @@
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1769,7 +1808,7 @@
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1786,7 +1825,7 @@
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1803,7 +1842,7 @@
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1839,7 +1878,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1849,14 +1888,14 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>39</v>
       </c>
@@ -1888,7 +1927,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>32</v>
       </c>
@@ -1914,7 +1953,7 @@
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>31</v>
       </c>
@@ -1940,7 +1979,7 @@
       <c r="I3" s="23"/>
       <c r="J3" s="23"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>33</v>
       </c>
@@ -1975,7 +2014,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>38</v>
       </c>
@@ -1991,7 +2030,7 @@
       <c r="I5" s="23"/>
       <c r="J5" s="23"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C9">
         <v>0.04</v>
       </c>
@@ -1999,7 +2038,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C10">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -2014,13 +2053,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update IO Assignments and controller layout
</commit_message>
<xml_diff>
--- a/IO Assignment.xlsx
+++ b/IO Assignment.xlsx
@@ -18,8 +18,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>CSC</author>
+  </authors>
+  <commentList>
+    <comment ref="E19" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>CSC:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Maybe able to use same solenoid as PTO
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="76">
   <si>
     <t>PWM Outputs</t>
   </si>
@@ -39,9 +74,6 @@
     <t>Left Encoder B</t>
   </si>
   <si>
-    <t>Solenoid Outputs</t>
-  </si>
-  <si>
     <t>Shifter</t>
   </si>
   <si>
@@ -222,9 +254,6 @@
     <t>Pickup</t>
   </si>
   <si>
-    <t>Climber Deploy</t>
-  </si>
-  <si>
     <t>PTO</t>
   </si>
   <si>
@@ -234,17 +263,32 @@
     <t>Climber Break</t>
   </si>
   <si>
-    <t>Frizbie Dump</t>
-  </si>
-  <si>
-    <t>Frizbie Flip</t>
+    <t>Shooter Pin</t>
+  </si>
+  <si>
+    <t>Shooter Feed</t>
+  </si>
+  <si>
+    <t>Shooter Elevation</t>
+  </si>
+  <si>
+    <t>Solenoid Outputs 2</t>
+  </si>
+  <si>
+    <t>Climber Deploy Out</t>
+  </si>
+  <si>
+    <t>Climber Deploy In</t>
+  </si>
+  <si>
+    <t>Solenoid Outputs 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,6 +307,19 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -291,7 +348,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -488,22 +545,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -557,7 +603,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -884,7 +929,7 @@
   <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -892,7 +937,7 @@
     <col min="1" max="1" width="3.19921875" customWidth="1"/>
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" customWidth="1"/>
-    <col min="5" max="5" width="16.19921875" customWidth="1"/>
+    <col min="5" max="5" width="17.69921875" customWidth="1"/>
     <col min="7" max="7" width="3.5" customWidth="1"/>
     <col min="8" max="8" width="12.59765625" customWidth="1"/>
     <col min="10" max="10" width="2.8984375" style="1" customWidth="1"/>
@@ -903,23 +948,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="22.8">
-      <c r="A1" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
+      <c r="A1" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="2"/>
@@ -956,30 +1001,30 @@
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="27"/>
+      <c r="D4" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="26"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="27"/>
+      <c r="G4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="26"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="27"/>
+      <c r="J4" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="26"/>
       <c r="L4" s="8"/>
-      <c r="M4" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" s="29"/>
+      <c r="M4" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="28"/>
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15">
@@ -987,30 +1032,30 @@
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="4">
         <v>1</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="4">
         <v>1</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="9"/>
       <c r="M5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N5" s="5"/>
       <c r="O5" s="2"/>
@@ -1020,35 +1065,35 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="4">
         <v>2</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="4">
         <v>2</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O6" s="2"/>
     </row>
@@ -1057,21 +1102,21 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="4">
         <v>3</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="4">
         <v>3</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="4">
@@ -1090,7 +1135,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="4">
@@ -1104,7 +1149,7 @@
         <v>4</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="4">
@@ -1123,14 +1168,14 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="4">
         <v>5</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="4">
@@ -1142,14 +1187,14 @@
         <v>3</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L9" s="9"/>
       <c r="M9" s="4">
         <v>3</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O9" s="2"/>
     </row>
@@ -1158,14 +1203,14 @@
         <v>6</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="4">
         <v>6</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="4">
@@ -1189,14 +1234,14 @@
         <v>7</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="4">
         <v>7</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="4">
@@ -1216,15 +1261,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="6">
         <v>8</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="E12" s="5"/>
       <c r="F12" s="2"/>
       <c r="G12" s="6">
         <v>8</v>
@@ -1243,7 +1286,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1296,25 +1339,25 @@
       <c r="O15" s="2"/>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="27"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="27"/>
+      <c r="D16" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="26"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="27"/>
+      <c r="G16" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="26"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="K16" s="32"/>
+      <c r="J16" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" s="31"/>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
@@ -1325,25 +1368,25 @@
         <v>1</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="4">
         <v>1</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="4">
         <v>1</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="9"/>
@@ -1362,7 +1405,9 @@
       <c r="D18" s="4">
         <v>2</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="E18" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="4">
         <v>2</v>
@@ -1370,7 +1415,7 @@
       <c r="H18" s="5"/>
       <c r="I18" s="2"/>
       <c r="J18" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="9"/>
@@ -1389,7 +1434,9 @@
       <c r="D19" s="4">
         <v>3</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="E19" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="4">
         <v>3</v>
@@ -1397,7 +1444,7 @@
       <c r="H19" s="5"/>
       <c r="I19" s="2"/>
       <c r="J19" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="2"/>
@@ -1424,7 +1471,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="2"/>
       <c r="J20" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K20" s="5"/>
       <c r="L20" s="10"/>
@@ -1457,12 +1504,12 @@
       <c r="N21" s="9"/>
       <c r="O21" s="2"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" ht="14.4" thickBot="1">
       <c r="A22" s="4">
         <v>6</v>
       </c>
-      <c r="B22" s="25" t="s">
-        <v>62</v>
+      <c r="B22" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="4">
@@ -1486,8 +1533,8 @@
       <c r="A23" s="4">
         <v>7</v>
       </c>
-      <c r="B23" s="25" t="s">
-        <v>63</v>
+      <c r="B23" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="4">
@@ -1495,8 +1542,10 @@
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="G23" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="26"/>
       <c r="I23" s="2"/>
       <c r="J23" s="4">
         <v>3</v>
@@ -1511,17 +1560,21 @@
       <c r="A24" s="4">
         <v>8</v>
       </c>
-      <c r="B24" s="25" t="s">
-        <v>64</v>
+      <c r="B24" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="6">
         <v>8</v>
       </c>
-      <c r="E24" s="7"/>
+      <c r="E24" s="5"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+      <c r="G24" s="4">
+        <v>1</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="I24" s="2"/>
       <c r="J24" s="4">
         <v>4</v>
@@ -1536,15 +1589,17 @@
       <c r="A25" s="4">
         <v>9</v>
       </c>
-      <c r="B25" s="25" t="s">
-        <v>65</v>
+      <c r="B25" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
+      <c r="G25" s="4">
+        <v>2</v>
+      </c>
+      <c r="H25" s="5"/>
       <c r="I25" s="2"/>
       <c r="J25" s="4">
         <v>5</v>
@@ -1560,14 +1615,16 @@
         <v>10</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="G26" s="4">
+        <v>3</v>
+      </c>
+      <c r="H26" s="5"/>
       <c r="I26" s="2"/>
       <c r="J26" s="4">
         <v>6</v>
@@ -1583,14 +1640,16 @@
         <v>11</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
+      <c r="G27" s="4">
+        <v>4</v>
+      </c>
+      <c r="H27" s="5"/>
       <c r="I27" s="2"/>
       <c r="J27" s="4">
         <v>7</v>
@@ -1607,13 +1666,15 @@
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28" s="32"/>
+      <c r="D28" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="31"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="G28" s="4">
+        <v>5</v>
+      </c>
+      <c r="H28" s="5"/>
       <c r="I28" s="2"/>
       <c r="J28" s="4">
         <v>8</v>
@@ -1634,11 +1695,13 @@
         <v>1</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
+      <c r="G29" s="4">
+        <v>6</v>
+      </c>
+      <c r="H29" s="5"/>
       <c r="I29" s="2"/>
       <c r="J29" s="4">
         <v>9</v>
@@ -1660,8 +1723,10 @@
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
+      <c r="G30" s="4">
+        <v>7</v>
+      </c>
+      <c r="H30" s="5"/>
       <c r="I30" s="2"/>
       <c r="J30" s="4">
         <v>10</v>
@@ -1681,8 +1746,10 @@
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
+      <c r="G31" s="6">
+        <v>8</v>
+      </c>
+      <c r="H31" s="7"/>
       <c r="I31" s="2"/>
       <c r="J31" s="11">
         <v>11</v>
@@ -1694,10 +1761,10 @@
       <c r="O31" s="2"/>
     </row>
     <row r="32" spans="1:15" ht="14.4" thickBot="1">
-      <c r="A32" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="27"/>
+      <c r="A32" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="26"/>
       <c r="C32" s="2"/>
       <c r="D32" s="4">
         <v>4</v>
@@ -1721,7 +1788,7 @@
         <v>1</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="4">
@@ -1901,7 +1968,7 @@
       <c r="O42" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="M4:N4"/>
@@ -1909,14 +1976,16 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="G23:H23"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="79" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="78" orientation="landscape" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1940,39 +2009,39 @@
   <sheetData>
     <row r="1" spans="1:11" ht="14.4" thickBot="1">
       <c r="A1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="19" t="s">
-        <v>47</v>
-      </c>
       <c r="J1" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="17">
         <v>2</v>
@@ -1987,7 +2056,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G2" s="17">
         <v>360</v>
@@ -1998,7 +2067,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="15">
         <v>3</v>
@@ -2013,7 +2082,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" s="15">
         <v>360</v>
@@ -2024,7 +2093,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="15">
         <v>4</v>
@@ -2039,7 +2108,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G4" s="15">
         <v>1408</v>
@@ -2054,12 +2123,12 @@
         <v>2112</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="15">
         <v>6</v>

</xml_diff>

<commit_message>
Changes to shooter code to account for new elevation modes
</commit_message>
<xml_diff>
--- a/IO Assignment.xlsx
+++ b/IO Assignment.xlsx
@@ -30,43 +30,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>CSC</author>
-  </authors>
-  <commentList>
-    <comment ref="E19" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>CSC:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Maybe able to use same solenoid as PTO
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="116">
   <si>
     <t>PWM Outputs</t>
   </si>
@@ -147,9 +112,6 @@
   </si>
   <si>
     <t>Piviot Omni</t>
-  </si>
-  <si>
-    <t>Omni</t>
   </si>
   <si>
     <t>CAN</t>
@@ -263,16 +225,7 @@
     <t>Shooter2 Encoder B</t>
   </si>
   <si>
-    <t>Pickup</t>
-  </si>
-  <si>
     <t>PTO</t>
-  </si>
-  <si>
-    <t>Pickup Deploy</t>
-  </si>
-  <si>
-    <t>Climber Break</t>
   </si>
   <si>
     <t>Shooter Pin</t>
@@ -432,7 +385,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -451,19 +404,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -5263,23 +5203,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="61729408"/>
-        <c:axId val="72995200"/>
+        <c:axId val="112675456"/>
+        <c:axId val="69505408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61729408"/>
+        <c:axId val="112675456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72995200"/>
+        <c:crossAx val="69505408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72995200"/>
+        <c:axId val="69505408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5287,7 +5227,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61729408"/>
+        <c:crossAx val="112675456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6804,22 +6744,22 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="71843840"/>
-        <c:axId val="71845376"/>
+        <c:axId val="70529024"/>
+        <c:axId val="70530560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71843840"/>
+        <c:axId val="70529024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71845376"/>
+        <c:crossAx val="70530560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71845376"/>
+        <c:axId val="70530560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6827,7 +6767,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71843840"/>
+        <c:crossAx val="70529024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8344,22 +8284,22 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="73037696"/>
-        <c:axId val="73039232"/>
+        <c:axId val="70600576"/>
+        <c:axId val="70602112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73037696"/>
+        <c:axId val="70600576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73039232"/>
+        <c:crossAx val="70602112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73039232"/>
+        <c:axId val="70602112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8367,7 +8307,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73037696"/>
+        <c:crossAx val="70600576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8785,7 +8725,7 @@
   <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -8805,7 +8745,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="23.25">
       <c r="A1" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -8863,7 +8803,7 @@
       <c r="B4" s="28"/>
       <c r="C4" s="2"/>
       <c r="D4" s="27" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E4" s="28"/>
       <c r="F4" s="2"/>
@@ -8888,7 +8828,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="4">
@@ -8902,7 +8842,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="4" t="s">
@@ -8921,21 +8861,21 @@
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="4">
         <v>2</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="4">
         <v>2</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="4" t="s">
@@ -8958,21 +8898,19 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="4">
         <v>3</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="E7" s="5"/>
       <c r="F7" s="2"/>
       <c r="G7" s="4">
         <v>3</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="4">
@@ -8991,21 +8929,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="4">
         <v>4</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="4">
         <v>4</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="4">
@@ -9024,14 +8962,14 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="4">
         <v>5</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="4">
@@ -9059,14 +8997,14 @@
         <v>6</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="4">
         <v>6</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="4">
@@ -9090,14 +9028,14 @@
         <v>7</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="4">
         <v>7</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="4">
@@ -9117,14 +9055,14 @@
         <v>8</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="6">
         <v>8</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="6">
@@ -9143,9 +9081,7 @@
       <c r="A13" s="4">
         <v>9</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>65</v>
-      </c>
+      <c r="B13" s="5"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -9203,7 +9139,7 @@
       <c r="B16" s="28"/>
       <c r="C16" s="2"/>
       <c r="D16" s="27" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E16" s="28"/>
       <c r="F16" s="2"/>
@@ -9255,7 +9191,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="4">
@@ -9282,15 +9218,13 @@
         <v>3</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="4">
         <v>3</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>68</v>
-      </c>
+      <c r="E19" s="5"/>
       <c r="F19" s="2"/>
       <c r="G19" s="4">
         <v>3</v>
@@ -9311,15 +9245,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="4">
         <v>4</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>67</v>
-      </c>
+      <c r="E20" s="5"/>
       <c r="F20" s="2"/>
       <c r="G20" s="4">
         <v>4</v>
@@ -9340,7 +9272,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="4">
@@ -9365,7 +9297,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="4">
@@ -9390,7 +9322,7 @@
         <v>7</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="4">
@@ -9417,7 +9349,7 @@
         <v>8</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="6">
@@ -9446,7 +9378,7 @@
         <v>9</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -9471,7 +9403,7 @@
         <v>10</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -9496,7 +9428,7 @@
         <v>11</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -9523,7 +9455,7 @@
       <c r="B28" s="5"/>
       <c r="C28" s="2"/>
       <c r="D28" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E28" s="33"/>
       <c r="F28" s="2"/>
@@ -9551,7 +9483,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="4">
@@ -9841,7 +9773,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="78" orientation="landscape" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -9865,39 +9796,39 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1">
       <c r="A1" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="19" t="s">
-        <v>46</v>
-      </c>
       <c r="J1" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="17">
         <v>2</v>
@@ -9912,7 +9843,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G2" s="17">
         <v>360</v>
@@ -9923,7 +9854,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="15">
         <v>3</v>
@@ -9938,7 +9869,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G3" s="15">
         <v>360</v>
@@ -9949,7 +9880,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="15">
         <v>4</v>
@@ -9964,7 +9895,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G4" s="15">
         <v>1408</v>
@@ -9979,12 +9910,12 @@
         <v>2112</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="15">
         <v>6</v>
@@ -10039,13 +9970,13 @@
   <sheetData>
     <row r="2" spans="1:10">
       <c r="B2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D2">
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F2">
         <f>PI()*D2</f>
@@ -10054,44 +9985,44 @@
     </row>
     <row r="3" spans="1:10">
       <c r="B3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D3">
         <v>128</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="28.5">
       <c r="B7" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="E7" t="s">
         <v>80</v>
       </c>
-      <c r="D7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E7" t="s">
-        <v>84</v>
-      </c>
       <c r="F7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B8">
         <v>613.64</v>
@@ -10126,7 +10057,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B9">
         <v>270</v>
@@ -10179,40 +10110,40 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B1">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D1">
         <v>0.05</v>
       </c>
       <c r="E1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F1">
         <v>36</v>
       </c>
       <c r="H1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I1">
         <v>0.02</v>
       </c>
       <c r="J1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="M1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="N1">
         <v>0.12</v>
       </c>
       <c r="O1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="P1">
         <v>0.05</v>
@@ -10220,40 +10151,40 @@
     </row>
     <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <v>0.01</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D2">
         <v>0.01</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I2">
         <v>4.5</v>
       </c>
       <c r="J2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="M2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
       <c r="O2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="P2">
         <v>0.01</v>
@@ -10261,31 +10192,31 @@
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D3">
         <v>2E-3</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F3">
         <v>0.5</v>
       </c>
       <c r="M3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="N3">
         <v>0</v>
       </c>
       <c r="O3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="P3">
         <v>2E-3</v>
@@ -10293,7 +10224,7 @@
     </row>
     <row r="5" spans="1:21" ht="28.5">
       <c r="B5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -10302,52 +10233,52 @@
         <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F5" t="s">
-        <v>103</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I5" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="M5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="P5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="T5" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="U5" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -46638,7 +46569,7 @@
         <v>449</v>
       </c>
       <c r="B454">
-        <f t="shared" ref="B454:B517" si="158">A454*Ts</f>
+        <f t="shared" ref="B454:B494" si="158">A454*Ts</f>
         <v>8.98</v>
       </c>
       <c r="C454" s="1">
@@ -46686,7 +46617,7 @@
         <v>0</v>
       </c>
       <c r="N454" s="1">
-        <f t="shared" ref="N454:N517" si="159">IF(H454&lt;2,0,K454*Sp +L454*Si + M454*Sd)</f>
+        <f t="shared" ref="N454:N494" si="159">IF(H454&lt;2,0,K454*Sp +L454*Si + M454*Sd)</f>
         <v>0</v>
       </c>
       <c r="O454" s="1">
@@ -46702,7 +46633,7 @@
         <v>0</v>
       </c>
       <c r="R454" s="1">
-        <f t="shared" ref="R454:R517" si="160">IF(H454&lt;2,0,MIN(O454*Dp +P454*Di + Q454*Dd,1)*Speed)</f>
+        <f t="shared" ref="R454:R494" si="160">IF(H454&lt;2,0,MIN(O454*Dp +P454*Di + Q454*Dd,1)*Speed)</f>
         <v>0</v>
       </c>
       <c r="T454">

</xml_diff>